<commit_message>
updated bill of material Microcontroller
</commit_message>
<xml_diff>
--- a/Production/Microcontroller_Submodule_BOM.xlsx
+++ b/Production/Microcontroller_Submodule_BOM.xlsx
@@ -8,24 +8,32 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sthab\Documents\EEE3088F\EEE3088F Project\Production\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1255DF6C-9D10-42B5-892D-B83F7B881350}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3F09E88C-EBCD-4912-8264-EE6376A73AA5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="28">
   <si>
     <t>100nF</t>
   </si>
@@ -48,21 +56,6 @@
     <t>$0.006</t>
   </si>
   <si>
-    <t xml:space="preserve">    U1</t>
-  </si>
-  <si>
-    <t>OPAMP</t>
-  </si>
-  <si>
-    <t>GS8092-SR</t>
-  </si>
-  <si>
-    <t>$0.4799</t>
-  </si>
-  <si>
-    <t xml:space="preserve">    U2</t>
-  </si>
-  <si>
     <t>AT24C256C-SSHL-T EEPROM</t>
   </si>
   <si>
@@ -72,9 +65,6 @@
     <t>$1.5556</t>
   </si>
   <si>
-    <t xml:space="preserve">    U3</t>
-  </si>
-  <si>
     <t>STM32F030C8Tx</t>
   </si>
   <si>
@@ -97,6 +87,36 @@
   </si>
   <si>
     <t>Qty</t>
+  </si>
+  <si>
+    <t>C254109</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    EEPROM1</t>
+  </si>
+  <si>
+    <t>AT24C256C-SSHL-T</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    MCU1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    OP-AMP1</t>
+  </si>
+  <si>
+    <t>LM358DT</t>
+  </si>
+  <si>
+    <t>C9418</t>
+  </si>
+  <si>
+    <t>$0.1043</t>
+  </si>
+  <si>
+    <t>C425317</t>
+  </si>
+  <si>
+    <t>Total = $1.6892</t>
   </si>
 </sst>
 </file>
@@ -152,14 +172,14 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{7903D17F-8700-4C27-A81E-9D9F5C0BA07A}" name="Table1" displayName="Table1" ref="A1:E6" totalsRowShown="0">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{7903D17F-8700-4C27-A81E-9D9F5C0BA07A}" name="Table1" displayName="Table1" ref="A1:E7" totalsRowCount="1">
   <autoFilter ref="A1:E6" xr:uid="{7903D17F-8700-4C27-A81E-9D9F5C0BA07A}"/>
   <tableColumns count="5">
     <tableColumn id="1" xr3:uid="{0F72FD48-95EC-4F07-91DE-B7F86ACB95E6}" name="Reference"/>
     <tableColumn id="2" xr3:uid="{309C3AB5-05AF-4440-9A97-6F346217C458}" name="Value"/>
     <tableColumn id="3" xr3:uid="{B7BFB3BC-D3B9-44C6-A3E1-EDD45295C651}" name="JLCPCB Part #"/>
     <tableColumn id="4" xr3:uid="{1165987F-3C28-4C19-9282-7EDCA1F04AAD}" name="Price"/>
-    <tableColumn id="5" xr3:uid="{07F5A22C-3E60-4A0E-A500-61275A3C4F05}" name="Qty"/>
+    <tableColumn id="5" xr3:uid="{07F5A22C-3E60-4A0E-A500-61275A3C4F05}" name="Qty" totalsRowLabel="Total = $1.6892"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight20" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -428,10 +448,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E6"/>
+  <dimension ref="A1:E7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G6" sqref="G6"/>
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -439,107 +459,109 @@
     <col min="1" max="1" width="21.81640625" customWidth="1"/>
     <col min="2" max="2" width="27.08984375" customWidth="1"/>
     <col min="3" max="3" width="25.26953125" customWidth="1"/>
-    <col min="4" max="4" width="18.6328125" customWidth="1"/>
-    <col min="5" max="5" width="10.26953125" customWidth="1"/>
+    <col min="4" max="4" width="23.81640625" customWidth="1"/>
+    <col min="5" max="5" width="21.90625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
-        <v>19</v>
+        <v>13</v>
       </c>
       <c r="B1" t="s">
-        <v>20</v>
+        <v>14</v>
       </c>
       <c r="C1" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="D1" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
       <c r="E1" t="s">
-        <v>23</v>
+        <v>17</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>18</v>
+        <v>12</v>
       </c>
       <c r="B2" t="s">
         <v>0</v>
       </c>
       <c r="C2" t="s">
+        <v>18</v>
+      </c>
+      <c r="D2" t="s">
         <v>1</v>
       </c>
-      <c r="D2" t="s">
-        <v>2</v>
-      </c>
-      <c r="E2">
+      <c r="E2" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>3</v>
+        <v>19</v>
       </c>
       <c r="B3" t="s">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="C3" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="D3" t="s">
-        <v>6</v>
-      </c>
-      <c r="E3">
-        <v>2</v>
+        <v>20</v>
+      </c>
+      <c r="E3" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>7</v>
+        <v>21</v>
       </c>
       <c r="B4" t="s">
-        <v>8</v>
-      </c>
-      <c r="C4" t="s">
-        <v>9</v>
-      </c>
-      <c r="D4" t="s">
         <v>10</v>
       </c>
-      <c r="E4">
-        <v>1</v>
+      <c r="E4" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>11</v>
+        <v>22</v>
       </c>
       <c r="B5" t="s">
-        <v>12</v>
+        <v>23</v>
       </c>
       <c r="C5" t="s">
-        <v>13</v>
+        <v>24</v>
       </c>
       <c r="D5" t="s">
-        <v>14</v>
-      </c>
-      <c r="E5">
-        <v>1</v>
+        <v>23</v>
+      </c>
+      <c r="E5" t="s">
+        <v>25</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>15</v>
+        <v>3</v>
       </c>
       <c r="B6" t="s">
-        <v>16</v>
+        <v>4</v>
+      </c>
+      <c r="C6" t="s">
+        <v>26</v>
       </c>
       <c r="D6" t="s">
-        <v>17</v>
-      </c>
-      <c r="E6">
-        <v>1</v>
+        <v>5</v>
+      </c>
+      <c r="E6" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="E7" t="s">
+        <v>27</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
updated microcontroller bill of material
</commit_message>
<xml_diff>
--- a/Production/Microcontroller_Submodule_BOM.xlsx
+++ b/Production/Microcontroller_Submodule_BOM.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sthab\Documents\EEE3088F\EEE3088F Project\Production\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3F09E88C-EBCD-4912-8264-EE6376A73AA5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2596A6A8-B686-4550-9AC0-9E10141A8C70}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -451,7 +451,7 @@
   <dimension ref="A1:E7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+      <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>

<commit_message>
updated bill of material
</commit_message>
<xml_diff>
--- a/Production/Microcontroller_Submodule_BOM.xlsx
+++ b/Production/Microcontroller_Submodule_BOM.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sthab\Documents\EEE3088F\EEE3088F Project\Production\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2596A6A8-B686-4550-9AC0-9E10141A8C70}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{876DCB49-02AB-495D-9587-69F99EBD8ABF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,31 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="28">
-  <si>
-    <t>100nF</t>
-  </si>
-  <si>
-    <t>CC2A104ZC1ID3F7C30MF</t>
-  </si>
-  <si>
-    <t>$0.0229</t>
-  </si>
-  <si>
-    <t>&gt;  R1, R2</t>
-  </si>
-  <si>
-    <t>33k</t>
-  </si>
-  <si>
-    <t>4D02WGF3302TCE</t>
-  </si>
-  <si>
-    <t>$0.006</t>
-  </si>
-  <si>
-    <t>AT24C256C-SSHL-T EEPROM</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="26">
   <si>
     <t>C6482</t>
   </si>
@@ -74,36 +50,21 @@
     <t>&gt;  C1, C2</t>
   </si>
   <si>
-    <t>Reference</t>
-  </si>
-  <si>
     <t>Value</t>
   </si>
   <si>
-    <t>JLCPCB Part #</t>
-  </si>
-  <si>
     <t>Price</t>
   </si>
   <si>
     <t>Qty</t>
   </si>
   <si>
-    <t>C254109</t>
-  </si>
-  <si>
-    <t xml:space="preserve">    EEPROM1</t>
-  </si>
-  <si>
     <t>AT24C256C-SSHL-T</t>
   </si>
   <si>
     <t xml:space="preserve">    MCU1</t>
   </si>
   <si>
-    <t xml:space="preserve">    OP-AMP1</t>
-  </si>
-  <si>
     <t>LM358DT</t>
   </si>
   <si>
@@ -113,16 +74,52 @@
     <t>$0.1043</t>
   </si>
   <si>
-    <t>C425317</t>
-  </si>
-  <si>
-    <t>Total = $1.6892</t>
+    <t>CL10A335KP8NNNC</t>
+  </si>
+  <si>
+    <t>$0.0143</t>
+  </si>
+  <si>
+    <t>C51412</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    IC1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    IC2</t>
+  </si>
+  <si>
+    <t>v  R1, R2</t>
+  </si>
+  <si>
+    <t>RC0603FR-071KL</t>
+  </si>
+  <si>
+    <t>$0.0012</t>
+  </si>
+  <si>
+    <t>C22548</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Reference </t>
+  </si>
+  <si>
+    <t>Manufacture Part Number</t>
+  </si>
+  <si>
+    <t>JLCPCB Part Number</t>
+  </si>
+  <si>
+    <t>total = $1.6782</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="6" formatCode="&quot;R&quot;#,##0;[Red]\-&quot;R&quot;#,##0"/>
+  </numFmts>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -132,12 +129,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -152,8 +155,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="6" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -172,16 +177,17 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{7903D17F-8700-4C27-A81E-9D9F5C0BA07A}" name="Table1" displayName="Table1" ref="A1:E7" totalsRowCount="1">
-  <autoFilter ref="A1:E6" xr:uid="{7903D17F-8700-4C27-A81E-9D9F5C0BA07A}"/>
-  <tableColumns count="5">
-    <tableColumn id="1" xr3:uid="{0F72FD48-95EC-4F07-91DE-B7F86ACB95E6}" name="Reference"/>
-    <tableColumn id="2" xr3:uid="{309C3AB5-05AF-4440-9A97-6F346217C458}" name="Value"/>
-    <tableColumn id="3" xr3:uid="{B7BFB3BC-D3B9-44C6-A3E1-EDD45295C651}" name="JLCPCB Part #"/>
-    <tableColumn id="4" xr3:uid="{1165987F-3C28-4C19-9282-7EDCA1F04AAD}" name="Price"/>
-    <tableColumn id="5" xr3:uid="{07F5A22C-3E60-4A0E-A500-61275A3C4F05}" name="Qty" totalsRowLabel="Total = $1.6892"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{08943F8D-2F81-4D22-9FD6-D3579747F0BF}" name="Table3" displayName="Table3" ref="A1:F9" totalsRowShown="0">
+  <autoFilter ref="A1:F9" xr:uid="{08943F8D-2F81-4D22-9FD6-D3579747F0BF}"/>
+  <tableColumns count="6">
+    <tableColumn id="1" xr3:uid="{0DCA09DC-0AB6-4914-8CA4-98E6F3592844}" name="Reference "/>
+    <tableColumn id="2" xr3:uid="{4DB74AD0-F1D6-4A9A-B59A-FDFEC63EA574}" name="Value"/>
+    <tableColumn id="3" xr3:uid="{6768D862-FFD4-4FDC-8E3C-0845104C0C04}" name="Manufacture Part Number"/>
+    <tableColumn id="4" xr3:uid="{98EF51F2-1250-4C19-A290-D43F87A81406}" name="Price"/>
+    <tableColumn id="5" xr3:uid="{EB8EE759-954E-4E79-8052-F7678190A6B5}" name="JLCPCB Part Number"/>
+    <tableColumn id="6" xr3:uid="{C9F72033-6D06-43A8-9789-49E779916CFD}" name="Qty"/>
   </tableColumns>
-  <tableStyleInfo name="TableStyleLight20" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
@@ -448,10 +454,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E7"/>
+  <dimension ref="A1:F9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+      <selection activeCell="E16" sqref="E16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -461,107 +467,166 @@
     <col min="3" max="3" width="25.26953125" customWidth="1"/>
     <col min="4" max="4" width="23.81640625" customWidth="1"/>
     <col min="5" max="5" width="21.90625" customWidth="1"/>
+    <col min="6" max="6" width="10.26953125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C1" t="s">
+        <v>23</v>
+      </c>
+      <c r="D1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E1" t="s">
+        <v>24</v>
+      </c>
+      <c r="F1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2" t="s">
         <v>13</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C2" t="s">
+        <v>13</v>
+      </c>
+      <c r="D2" t="s">
         <v>14</v>
       </c>
-      <c r="C1" t="s">
+      <c r="E2" t="s">
         <v>15</v>
       </c>
-      <c r="D1" t="s">
+      <c r="F2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
         <v>16</v>
       </c>
-      <c r="E1" t="s">
+      <c r="B3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D3" t="s">
+        <v>12</v>
+      </c>
+      <c r="E3" t="s">
+        <v>11</v>
+      </c>
+      <c r="F3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A2" t="s">
-        <v>12</v>
-      </c>
-      <c r="B2" t="s">
+      <c r="B4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C4" t="s">
+        <v>8</v>
+      </c>
+      <c r="D4" t="s">
+        <v>1</v>
+      </c>
+      <c r="E4" t="s">
         <v>0</v>
       </c>
-      <c r="C2" t="s">
+      <c r="F4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
+        <v>9</v>
+      </c>
+      <c r="B5" t="s">
+        <v>2</v>
+      </c>
+      <c r="D5" t="s">
+        <v>3</v>
+      </c>
+      <c r="F5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A6" t="s">
         <v>18</v>
       </c>
-      <c r="D2" t="s">
+      <c r="B6" t="s">
+        <v>19</v>
+      </c>
+      <c r="C6" t="s">
+        <v>19</v>
+      </c>
+      <c r="D6" t="s">
+        <v>20</v>
+      </c>
+      <c r="E6" t="s">
+        <v>21</v>
+      </c>
+      <c r="F6">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A7" s="1">
         <v>1</v>
       </c>
-      <c r="E2" t="s">
+      <c r="B7" t="s">
+        <v>19</v>
+      </c>
+      <c r="C7" t="s">
+        <v>19</v>
+      </c>
+      <c r="D7" t="s">
+        <v>20</v>
+      </c>
+      <c r="E7" t="s">
+        <v>21</v>
+      </c>
+      <c r="F7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A8" s="1">
         <v>2</v>
       </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A3" t="s">
+      <c r="B8" t="s">
         <v>19</v>
       </c>
-      <c r="B3" t="s">
-        <v>7</v>
-      </c>
-      <c r="C3" t="s">
-        <v>8</v>
-      </c>
-      <c r="D3" t="s">
+      <c r="C8" t="s">
+        <v>19</v>
+      </c>
+      <c r="D8" t="s">
         <v>20</v>
       </c>
-      <c r="E3" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A4" t="s">
+      <c r="E8" t="s">
         <v>21</v>
       </c>
-      <c r="B4" t="s">
-        <v>10</v>
-      </c>
-      <c r="E4" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A5" t="s">
-        <v>22</v>
-      </c>
-      <c r="B5" t="s">
-        <v>23</v>
-      </c>
-      <c r="C5" t="s">
-        <v>24</v>
-      </c>
-      <c r="D5" t="s">
-        <v>23</v>
-      </c>
-      <c r="E5" t="s">
+      <c r="F8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="D9" s="2" t="s">
         <v>25</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A6" t="s">
-        <v>3</v>
-      </c>
-      <c r="B6" t="s">
-        <v>4</v>
-      </c>
-      <c r="C6" t="s">
-        <v>26</v>
-      </c>
-      <c r="D6" t="s">
-        <v>5</v>
-      </c>
-      <c r="E6" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="E7" t="s">
-        <v>27</v>
       </c>
     </row>
   </sheetData>

</xml_diff>